<commit_message>
minor issue on empirical
</commit_message>
<xml_diff>
--- a/empirical.xlsx
+++ b/empirical.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huanghuaxun/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huanghuaxun/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="1340" windowWidth="26960" windowHeight="15380" tabRatio="500"/>
+    <workbookView xWindow="12220" yWindow="2840" windowWidth="26960" windowHeight="15380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="154">
   <si>
     <t>Project</t>
   </si>
@@ -453,6 +453,9 @@
     <t>89ebafe</t>
   </si>
   <si>
+    <t>satstat</t>
+  </si>
+  <si>
     <t>uhabits</t>
   </si>
   <si>
@@ -543,25 +546,10 @@
     <t>CCFG edge inconsistency</t>
   </si>
   <si>
-    <t>9c1217-</t>
-  </si>
-  <si>
-    <t>edx-android</t>
-  </si>
-  <si>
-    <t>9e82f4b</t>
-  </si>
-  <si>
-    <t>78b175f</t>
-  </si>
-  <si>
-    <t>vineYard</t>
-  </si>
-  <si>
-    <t>issue tracker</t>
-  </si>
-  <si>
-    <t>diff change</t>
+    <t xml:space="preserve"> VineYard</t>
+  </si>
+  <si>
+    <t>9c12170</t>
   </si>
 </sst>
 </file>
@@ -942,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -957,7 +945,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -989,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1003,13 +991,13 @@
         <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1023,13 +1011,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1043,13 +1031,13 @@
         <v>14</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1080,10 +1068,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1097,10 +1085,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1114,13 +1102,13 @@
         <v>19</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1134,10 +1122,10 @@
         <v>20</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1151,13 +1139,13 @@
         <v>21</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1174,10 +1162,10 @@
         <v>6</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1191,13 +1179,13 @@
         <v>24</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1211,10 +1199,10 @@
         <v>25</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1228,13 +1216,13 @@
         <v>27</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1248,10 +1236,10 @@
         <v>2.6800000000000002E+90</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1265,13 +1253,13 @@
         <v>30</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1285,13 +1273,13 @@
         <v>31</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1305,10 +1293,10 @@
         <v>33</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1322,10 +1310,10 @@
         <v>34</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1339,13 +1327,13 @@
         <v>36</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1359,10 +1347,10 @@
         <v>37</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1376,10 +1364,10 @@
         <v>37</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1387,19 +1375,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>153</v>
+        <v>38</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1407,19 +1395,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>154</v>
+        <v>40</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1427,19 +1415,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1447,19 +1435,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1467,19 +1455,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1487,19 +1475,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1507,19 +1495,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1530,16 +1518,16 @@
         <v>45</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1550,16 +1538,16 @@
         <v>45</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1570,13 +1558,13 @@
         <v>45</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1587,13 +1575,10 @@
         <v>45</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>145</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1604,16 +1589,16 @@
         <v>45</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1621,13 +1606,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>6</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1635,19 +1620,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1655,16 +1640,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1675,13 +1663,13 @@
         <v>56</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>149</v>
+        <v>6</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1692,16 +1680,16 @@
         <v>56</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1712,16 +1700,16 @@
         <v>56</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>6</v>
+        <v>150</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1732,13 +1720,10 @@
         <v>56</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>146</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1749,13 +1734,13 @@
         <v>56</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1766,13 +1751,16 @@
         <v>56</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>6</v>
+        <v>150</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1783,16 +1771,16 @@
         <v>56</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1800,16 +1788,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1817,19 +1802,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1840,13 +1825,16 @@
         <v>52</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1854,19 +1842,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1874,19 +1862,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>150</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1894,19 +1882,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E51" s="4" t="s">
-        <v>145</v>
-      </c>
       <c r="F51" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1914,19 +1899,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -1934,37 +1919,28 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>75</v>
+        <v>63</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>146</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>146</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
@@ -1973,33 +1949,31 @@
       <c r="B55" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>64</v>
+      <c r="C55" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
+        <v>150</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -2007,13 +1981,19 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -2021,19 +2001,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2041,16 +2021,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F59" s="4" t="s">
         <v>146</v>
@@ -2064,16 +2044,13 @@
         <v>85</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2081,16 +2058,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -2098,19 +2078,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="C62" s="6">
+        <v>8.6600000000000008E+37</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -2120,17 +2100,17 @@
       <c r="B63" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C63" s="6">
-        <v>8.6600000000000008E+37</v>
+      <c r="C63" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2138,19 +2118,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D64" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E64" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2158,16 +2135,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D65" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F65" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -2178,16 +2158,10 @@
         <v>95</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -2198,10 +2172,13 @@
         <v>95</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>150</v>
+        <v>6</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -2212,13 +2189,13 @@
         <v>95</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -2226,16 +2203,16 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>6</v>
+        <v>150</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -2243,16 +2220,19 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2260,19 +2240,19 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2283,16 +2263,10 @@
         <v>91</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -2303,10 +2277,16 @@
         <v>91</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2317,16 +2297,10 @@
         <v>91</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2334,19 +2308,19 @@
         <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2354,19 +2328,16 @@
         <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F76" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -2377,13 +2348,16 @@
         <v>110</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2391,19 +2365,16 @@
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2414,13 +2385,13 @@
         <v>113</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -2428,16 +2399,19 @@
         <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -2448,16 +2422,10 @@
         <v>118</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F81" s="4" t="s">
-        <v>145</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -2465,16 +2433,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
+      </c>
+      <c r="C82" s="4">
+        <v>4431454</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E82" s="4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -2482,16 +2447,16 @@
         <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -2499,19 +2464,19 @@
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -2519,16 +2484,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -2542,13 +2504,13 @@
         <v>2264346</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -2559,16 +2521,16 @@
         <v>115</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -2579,13 +2541,13 @@
         <v>115</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -2596,13 +2558,13 @@
         <v>117</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -2610,16 +2572,16 @@
         <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -2627,19 +2589,19 @@
         <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -2647,19 +2609,19 @@
         <v>91</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -2667,16 +2629,16 @@
         <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F93" s="4"/>
     </row>
@@ -2685,19 +2647,19 @@
         <v>93</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -2705,19 +2667,19 @@
         <v>94</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -2725,16 +2687,16 @@
         <v>95</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -2742,16 +2704,16 @@
         <v>96</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -2759,19 +2721,19 @@
         <v>97</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
@@ -2779,19 +2741,19 @@
         <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
@@ -2799,16 +2761,16 @@
         <v>99</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
@@ -2816,19 +2778,19 @@
         <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -2996,8 +2958,8 @@
     </row>
   </sheetData>
   <autoFilter ref="B1:E101">
-    <sortState ref="B2:E101">
-      <sortCondition ref="B1:B101"/>
+    <sortState ref="B2:F101">
+      <sortCondition ref="B2"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -3021,233 +2983,226 @@
     <hyperlink ref="C21" r:id="rId18"/>
     <hyperlink ref="C22" r:id="rId19"/>
     <hyperlink ref="C23" r:id="rId20"/>
-    <hyperlink ref="C26" r:id="rId21"/>
-    <hyperlink ref="C27" r:id="rId22"/>
-    <hyperlink ref="C29" r:id="rId23"/>
-    <hyperlink ref="C30" r:id="rId24"/>
-    <hyperlink ref="C31" r:id="rId25"/>
-    <hyperlink ref="C32" r:id="rId26"/>
-    <hyperlink ref="C33" r:id="rId27"/>
-    <hyperlink ref="C34" r:id="rId28"/>
-    <hyperlink ref="C35" r:id="rId29"/>
-    <hyperlink ref="C36" r:id="rId30"/>
-    <hyperlink ref="C37" r:id="rId31"/>
-    <hyperlink ref="C38" r:id="rId32"/>
-    <hyperlink ref="C39" r:id="rId33"/>
-    <hyperlink ref="C40" r:id="rId34"/>
-    <hyperlink ref="C41" r:id="rId35"/>
-    <hyperlink ref="C42" r:id="rId36"/>
-    <hyperlink ref="C43" r:id="rId37"/>
-    <hyperlink ref="C44" r:id="rId38"/>
-    <hyperlink ref="C45" r:id="rId39"/>
-    <hyperlink ref="C46" r:id="rId40"/>
-    <hyperlink ref="C47" r:id="rId41"/>
-    <hyperlink ref="C48" r:id="rId42"/>
-    <hyperlink ref="C49" r:id="rId43"/>
-    <hyperlink ref="C50" r:id="rId44"/>
-    <hyperlink ref="C51" r:id="rId45"/>
-    <hyperlink ref="C52" r:id="rId46"/>
-    <hyperlink ref="C53" r:id="rId47"/>
-    <hyperlink ref="C56" r:id="rId48"/>
-    <hyperlink ref="C57" r:id="rId49"/>
-    <hyperlink ref="C58" r:id="rId50"/>
-    <hyperlink ref="C59" r:id="rId51"/>
-    <hyperlink ref="C60" r:id="rId52"/>
-    <hyperlink ref="C61" r:id="rId53"/>
-    <hyperlink ref="C62" r:id="rId54"/>
-    <hyperlink ref="C63" r:id="rId55" display="https://github.com/samuelclay/NewsBlur/commit/0866e35b9c2d116ebd13878da3b63b5147d7e26b"/>
-    <hyperlink ref="C64" r:id="rId56"/>
-    <hyperlink ref="C65" r:id="rId57"/>
-    <hyperlink ref="C66" r:id="rId58"/>
-    <hyperlink ref="C67" r:id="rId59"/>
-    <hyperlink ref="C68" r:id="rId60"/>
-    <hyperlink ref="C69" r:id="rId61"/>
-    <hyperlink ref="C70" r:id="rId62"/>
-    <hyperlink ref="C71" r:id="rId63"/>
-    <hyperlink ref="C72" r:id="rId64"/>
-    <hyperlink ref="C74" r:id="rId65"/>
-    <hyperlink ref="C75" r:id="rId66"/>
-    <hyperlink ref="C76" r:id="rId67"/>
-    <hyperlink ref="C77" r:id="rId68"/>
-    <hyperlink ref="C78" r:id="rId69"/>
-    <hyperlink ref="C79" r:id="rId70"/>
-    <hyperlink ref="C80" r:id="rId71"/>
-    <hyperlink ref="C81" r:id="rId72"/>
-    <hyperlink ref="C82" r:id="rId73"/>
-    <hyperlink ref="C92" r:id="rId74"/>
-    <hyperlink ref="C83" r:id="rId75"/>
-    <hyperlink ref="C84" r:id="rId76"/>
-    <hyperlink ref="C85" r:id="rId77"/>
-    <hyperlink ref="C86" r:id="rId78" display="https://github.com/bottiger/SoundWaves/commit/2264346bda29ffd762aca3eeb88deb765deb9081"/>
-    <hyperlink ref="C87" r:id="rId79"/>
-    <hyperlink ref="C88" r:id="rId80"/>
-    <hyperlink ref="C90" r:id="rId81"/>
-    <hyperlink ref="C91" r:id="rId82"/>
-    <hyperlink ref="C94" r:id="rId83"/>
-    <hyperlink ref="C95" r:id="rId84"/>
-    <hyperlink ref="C96" r:id="rId85"/>
-    <hyperlink ref="C97" r:id="rId86"/>
-    <hyperlink ref="C98" r:id="rId87"/>
-    <hyperlink ref="C99" r:id="rId88"/>
-    <hyperlink ref="C100" r:id="rId89"/>
-    <hyperlink ref="C101" r:id="rId90"/>
-    <hyperlink ref="C28" r:id="rId91"/>
-    <hyperlink ref="C5" r:id="rId92"/>
-    <hyperlink ref="C73" r:id="rId93"/>
-    <hyperlink ref="C89" r:id="rId94"/>
-    <hyperlink ref="E4" r:id="rId95" location="onattach"/>
-    <hyperlink ref="E5" r:id="rId96" location="onattach"/>
-    <hyperlink ref="E47" r:id="rId97" location="onattach"/>
-    <hyperlink ref="E54" r:id="rId98" location="onattach"/>
-    <hyperlink ref="E62" r:id="rId99" location="onattach"/>
-    <hyperlink ref="E72" r:id="rId100" location="onattach"/>
-    <hyperlink ref="E86" r:id="rId101" location="onattach"/>
-    <hyperlink ref="E91" r:id="rId102" location="onattach"/>
-    <hyperlink ref="E95" r:id="rId103" location="onattach"/>
-    <hyperlink ref="E98" r:id="rId104" location="onattach"/>
-    <hyperlink ref="E101" r:id="rId105" location="onattach"/>
-    <hyperlink ref="F4" r:id="rId106"/>
-    <hyperlink ref="F5" r:id="rId107"/>
-    <hyperlink ref="F45" r:id="rId108"/>
-    <hyperlink ref="F52" r:id="rId109"/>
-    <hyperlink ref="F62" r:id="rId110"/>
-    <hyperlink ref="F72" r:id="rId111"/>
-    <hyperlink ref="F86" r:id="rId112"/>
-    <hyperlink ref="F91" r:id="rId113"/>
-    <hyperlink ref="F95" r:id="rId114"/>
-    <hyperlink ref="F98" r:id="rId115"/>
-    <hyperlink ref="F101" r:id="rId116"/>
-    <hyperlink ref="E3" r:id="rId117" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E13" r:id="rId118" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E15" r:id="rId119" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E26" r:id="rId120" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E27" r:id="rId121" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E52" r:id="rId122" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E58" r:id="rId123" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E60" r:id="rId124" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E71" r:id="rId125" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E78" r:id="rId126" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E81" r:id="rId127" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E87" r:id="rId128" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E92" r:id="rId129" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E94" r:id="rId130" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E76" r:id="rId131" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E43" r:id="rId132" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E37" r:id="rId133" location="onrequestpermissionsresult"/>
-    <hyperlink ref="E34" r:id="rId134" location="onrequestpermissionsresult"/>
-    <hyperlink ref="F3" r:id="rId135"/>
-    <hyperlink ref="F13" r:id="rId136"/>
-    <hyperlink ref="F15" r:id="rId137"/>
-    <hyperlink ref="F24" r:id="rId138"/>
-    <hyperlink ref="F25" r:id="rId139"/>
-    <hyperlink ref="F32" r:id="rId140"/>
-    <hyperlink ref="F35" r:id="rId141"/>
-    <hyperlink ref="F41" r:id="rId142"/>
-    <hyperlink ref="F50" r:id="rId143"/>
-    <hyperlink ref="F58" r:id="rId144"/>
-    <hyperlink ref="F60" r:id="rId145"/>
-    <hyperlink ref="F71" r:id="rId146"/>
-    <hyperlink ref="F76" r:id="rId147"/>
-    <hyperlink ref="F78" r:id="rId148"/>
-    <hyperlink ref="F81" r:id="rId149"/>
-    <hyperlink ref="F92" r:id="rId150"/>
-    <hyperlink ref="F94" r:id="rId151"/>
-    <hyperlink ref="F87" r:id="rId152"/>
-    <hyperlink ref="F28" r:id="rId153" display="official doc"/>
-    <hyperlink ref="F30" r:id="rId154" display="official doc"/>
-    <hyperlink ref="F37" r:id="rId155" display="official doc"/>
-    <hyperlink ref="F63" r:id="rId156" display="official doc"/>
-    <hyperlink ref="E39" r:id="rId157" location="shouldoverrideurlloading"/>
-    <hyperlink ref="E30" r:id="rId158" location="shouldoverrideurlloading"/>
-    <hyperlink ref="E32" r:id="rId159" location="shouldoverrideurlloading"/>
-    <hyperlink ref="E63" r:id="rId160" location="shouldoverrideurlloading"/>
-    <hyperlink ref="E33" r:id="rId161" location="shouldinterceptrequest"/>
-    <hyperlink ref="E49" r:id="rId162" location="shouldinterceptrequest"/>
-    <hyperlink ref="E99" r:id="rId163" location="shouldinterceptrequest"/>
-    <hyperlink ref="F31" r:id="rId164"/>
-    <hyperlink ref="F99" r:id="rId165"/>
-    <hyperlink ref="F47" r:id="rId166"/>
-    <hyperlink ref="E9" r:id="rId167" location="onrequestpermissionsresult"/>
-    <hyperlink ref="F9" r:id="rId168"/>
-    <hyperlink ref="F27" r:id="rId169"/>
-    <hyperlink ref="F29" r:id="rId170"/>
-    <hyperlink ref="F44" r:id="rId171"/>
-    <hyperlink ref="F74" r:id="rId172"/>
-    <hyperlink ref="F84" r:id="rId173"/>
-    <hyperlink ref="E29" r:id="rId174" location="onreceivederror"/>
-    <hyperlink ref="E31" r:id="rId175" location="onreceivederror"/>
-    <hyperlink ref="E46" r:id="rId176" location="onreceivederror"/>
-    <hyperlink ref="E74" r:id="rId177" location="onreceivederror"/>
-    <hyperlink ref="E84" r:id="rId178" location="onreceivederror"/>
-    <hyperlink ref="E22" r:id="rId179" location="onResume()"/>
-    <hyperlink ref="E23" r:id="rId180" location="onPause()"/>
-    <hyperlink ref="E17" r:id="rId181" location="onlowmemory"/>
-    <hyperlink ref="E28" r:id="rId182" location="onlowmemory"/>
-    <hyperlink ref="E59" r:id="rId183" location="onlowmemory"/>
-    <hyperlink ref="F17" r:id="rId184"/>
-    <hyperlink ref="F26" r:id="rId185"/>
-    <hyperlink ref="F59" r:id="rId186"/>
-    <hyperlink ref="E56" r:id="rId187" location="onrequestpermissionsresult"/>
-    <hyperlink ref="F56" r:id="rId188"/>
-    <hyperlink ref="F11" r:id="rId189"/>
-    <hyperlink ref="F18" r:id="rId190"/>
-    <hyperlink ref="F48" r:id="rId191"/>
-    <hyperlink ref="F49" r:id="rId192"/>
-    <hyperlink ref="E2" r:id="rId193"/>
-    <hyperlink ref="E69" r:id="rId194"/>
+    <hyperlink ref="C24" r:id="rId21"/>
+    <hyperlink ref="C25" r:id="rId22"/>
+    <hyperlink ref="C27" r:id="rId23"/>
+    <hyperlink ref="C28" r:id="rId24"/>
+    <hyperlink ref="C29" r:id="rId25"/>
+    <hyperlink ref="C30" r:id="rId26"/>
+    <hyperlink ref="C31" r:id="rId27"/>
+    <hyperlink ref="C32" r:id="rId28"/>
+    <hyperlink ref="C33" r:id="rId29"/>
+    <hyperlink ref="C34" r:id="rId30"/>
+    <hyperlink ref="C35" r:id="rId31"/>
+    <hyperlink ref="C36" r:id="rId32"/>
+    <hyperlink ref="C37" r:id="rId33"/>
+    <hyperlink ref="C38" r:id="rId34"/>
+    <hyperlink ref="C39" r:id="rId35"/>
+    <hyperlink ref="C40" r:id="rId36"/>
+    <hyperlink ref="C41" r:id="rId37"/>
+    <hyperlink ref="C42" r:id="rId38"/>
+    <hyperlink ref="C43" r:id="rId39"/>
+    <hyperlink ref="C44" r:id="rId40"/>
+    <hyperlink ref="C45" r:id="rId41"/>
+    <hyperlink ref="C46" r:id="rId42"/>
+    <hyperlink ref="C47" r:id="rId43"/>
+    <hyperlink ref="C48" r:id="rId44"/>
+    <hyperlink ref="C49" r:id="rId45"/>
+    <hyperlink ref="C50" r:id="rId46"/>
+    <hyperlink ref="C51" r:id="rId47"/>
+    <hyperlink ref="C55" r:id="rId48"/>
+    <hyperlink ref="C56" r:id="rId49"/>
+    <hyperlink ref="C57" r:id="rId50"/>
+    <hyperlink ref="C58" r:id="rId51"/>
+    <hyperlink ref="C59" r:id="rId52"/>
+    <hyperlink ref="C60" r:id="rId53"/>
+    <hyperlink ref="C61" r:id="rId54"/>
+    <hyperlink ref="C62" r:id="rId55" display="https://github.com/samuelclay/NewsBlur/commit/0866e35b9c2d116ebd13878da3b63b5147d7e26b"/>
+    <hyperlink ref="C63" r:id="rId56"/>
+    <hyperlink ref="C64" r:id="rId57"/>
+    <hyperlink ref="C65" r:id="rId58"/>
+    <hyperlink ref="C66" r:id="rId59"/>
+    <hyperlink ref="C67" r:id="rId60"/>
+    <hyperlink ref="C68" r:id="rId61"/>
+    <hyperlink ref="C69" r:id="rId62"/>
+    <hyperlink ref="C70" r:id="rId63"/>
+    <hyperlink ref="C71" r:id="rId64"/>
+    <hyperlink ref="C73" r:id="rId65"/>
+    <hyperlink ref="C74" r:id="rId66"/>
+    <hyperlink ref="C75" r:id="rId67"/>
+    <hyperlink ref="C76" r:id="rId68"/>
+    <hyperlink ref="C77" r:id="rId69"/>
+    <hyperlink ref="C78" r:id="rId70"/>
+    <hyperlink ref="C79" r:id="rId71"/>
+    <hyperlink ref="C80" r:id="rId72"/>
+    <hyperlink ref="C81" r:id="rId73"/>
+    <hyperlink ref="C82" r:id="rId74" display="https://github.com/mvglasow/satstat/commit/44314543e591493d9fbe4aa765a831d8a5b5a6ba"/>
+    <hyperlink ref="C92" r:id="rId75"/>
+    <hyperlink ref="C83" r:id="rId76"/>
+    <hyperlink ref="C84" r:id="rId77"/>
+    <hyperlink ref="C85" r:id="rId78"/>
+    <hyperlink ref="C86" r:id="rId79" display="https://github.com/bottiger/SoundWaves/commit/2264346bda29ffd762aca3eeb88deb765deb9081"/>
+    <hyperlink ref="C87" r:id="rId80"/>
+    <hyperlink ref="C88" r:id="rId81"/>
+    <hyperlink ref="C90" r:id="rId82"/>
+    <hyperlink ref="C91" r:id="rId83"/>
+    <hyperlink ref="C94" r:id="rId84"/>
+    <hyperlink ref="C95" r:id="rId85"/>
+    <hyperlink ref="C96" r:id="rId86"/>
+    <hyperlink ref="C97" r:id="rId87"/>
+    <hyperlink ref="C98" r:id="rId88"/>
+    <hyperlink ref="C99" r:id="rId89"/>
+    <hyperlink ref="C100" r:id="rId90"/>
+    <hyperlink ref="C101" r:id="rId91"/>
+    <hyperlink ref="C26" r:id="rId92"/>
+    <hyperlink ref="C5" r:id="rId93"/>
+    <hyperlink ref="C72" r:id="rId94"/>
+    <hyperlink ref="C89" r:id="rId95"/>
+    <hyperlink ref="E4" r:id="rId96" location="onattach"/>
+    <hyperlink ref="E5" r:id="rId97" location="onattach"/>
+    <hyperlink ref="E45" r:id="rId98" location="onattach"/>
+    <hyperlink ref="E52" r:id="rId99" location="onattach"/>
+    <hyperlink ref="E61" r:id="rId100" location="onattach"/>
+    <hyperlink ref="E71" r:id="rId101" location="onattach"/>
+    <hyperlink ref="E86" r:id="rId102" location="onattach"/>
+    <hyperlink ref="E91" r:id="rId103" location="onattach"/>
+    <hyperlink ref="E95" r:id="rId104" location="onattach"/>
+    <hyperlink ref="E98" r:id="rId105" location="onattach"/>
+    <hyperlink ref="E101" r:id="rId106" location="onattach"/>
+    <hyperlink ref="F4" r:id="rId107"/>
+    <hyperlink ref="F5" r:id="rId108"/>
+    <hyperlink ref="F45" r:id="rId109"/>
+    <hyperlink ref="F52" r:id="rId110"/>
+    <hyperlink ref="F61" r:id="rId111"/>
+    <hyperlink ref="F71" r:id="rId112"/>
+    <hyperlink ref="F86" r:id="rId113"/>
+    <hyperlink ref="F91" r:id="rId114"/>
+    <hyperlink ref="F95" r:id="rId115"/>
+    <hyperlink ref="F98" r:id="rId116"/>
+    <hyperlink ref="F101" r:id="rId117"/>
+    <hyperlink ref="E3" r:id="rId118" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E13" r:id="rId119" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E15" r:id="rId120" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E24" r:id="rId121" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E25" r:id="rId122" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E50" r:id="rId123" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E57" r:id="rId124" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E59" r:id="rId125" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E70" r:id="rId126" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E77" r:id="rId127" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E80" r:id="rId128" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E87" r:id="rId129" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E92" r:id="rId130" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E94" r:id="rId131" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E75" r:id="rId132" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E41" r:id="rId133" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E35" r:id="rId134" location="onrequestpermissionsresult"/>
+    <hyperlink ref="E32" r:id="rId135" location="onrequestpermissionsresult"/>
+    <hyperlink ref="F3" r:id="rId136"/>
+    <hyperlink ref="F13" r:id="rId137"/>
+    <hyperlink ref="F15" r:id="rId138"/>
+    <hyperlink ref="F24" r:id="rId139"/>
+    <hyperlink ref="F25" r:id="rId140"/>
+    <hyperlink ref="F32" r:id="rId141"/>
+    <hyperlink ref="F35" r:id="rId142"/>
+    <hyperlink ref="F41" r:id="rId143"/>
+    <hyperlink ref="F50" r:id="rId144"/>
+    <hyperlink ref="F57" r:id="rId145"/>
+    <hyperlink ref="F59" r:id="rId146"/>
+    <hyperlink ref="F70" r:id="rId147"/>
+    <hyperlink ref="F75" r:id="rId148"/>
+    <hyperlink ref="F77" r:id="rId149"/>
+    <hyperlink ref="F80" r:id="rId150"/>
+    <hyperlink ref="F92" r:id="rId151"/>
+    <hyperlink ref="F94" r:id="rId152"/>
+    <hyperlink ref="F87" r:id="rId153"/>
+    <hyperlink ref="F28" r:id="rId154" display="official doc"/>
+    <hyperlink ref="F30" r:id="rId155" display="official doc"/>
+    <hyperlink ref="F37" r:id="rId156" display="official doc"/>
+    <hyperlink ref="F62" r:id="rId157" display="official doc"/>
+    <hyperlink ref="E37" r:id="rId158" location="shouldoverrideurlloading"/>
+    <hyperlink ref="E28" r:id="rId159" location="shouldoverrideurlloading"/>
+    <hyperlink ref="E30" r:id="rId160" location="shouldoverrideurlloading"/>
+    <hyperlink ref="E62" r:id="rId161" location="shouldoverrideurlloading"/>
+    <hyperlink ref="E31" r:id="rId162" location="shouldinterceptrequest"/>
+    <hyperlink ref="E47" r:id="rId163" location="shouldinterceptrequest"/>
+    <hyperlink ref="E99" r:id="rId164" location="shouldinterceptrequest"/>
+    <hyperlink ref="F31" r:id="rId165"/>
+    <hyperlink ref="F99" r:id="rId166"/>
+    <hyperlink ref="F47" r:id="rId167"/>
+    <hyperlink ref="E9" r:id="rId168" location="onrequestpermissionsresult"/>
+    <hyperlink ref="F9" r:id="rId169"/>
+    <hyperlink ref="F27" r:id="rId170"/>
+    <hyperlink ref="F29" r:id="rId171"/>
+    <hyperlink ref="F44" r:id="rId172"/>
+    <hyperlink ref="F73" r:id="rId173"/>
+    <hyperlink ref="F84" r:id="rId174"/>
+    <hyperlink ref="E27" r:id="rId175" location="onreceivederror"/>
+    <hyperlink ref="E29" r:id="rId176" location="onreceivederror"/>
+    <hyperlink ref="E44" r:id="rId177" location="onreceivederror"/>
+    <hyperlink ref="E73" r:id="rId178" location="onreceivederror"/>
+    <hyperlink ref="E84" r:id="rId179" location="onreceivederror"/>
+    <hyperlink ref="E22" r:id="rId180" location="onResume()"/>
+    <hyperlink ref="E23" r:id="rId181" location="onPause()"/>
+    <hyperlink ref="E17" r:id="rId182" location="onlowmemory"/>
+    <hyperlink ref="E26" r:id="rId183" location="onlowmemory"/>
+    <hyperlink ref="E58" r:id="rId184" location="onlowmemory"/>
+    <hyperlink ref="F17" r:id="rId185"/>
+    <hyperlink ref="F26" r:id="rId186"/>
+    <hyperlink ref="F58" r:id="rId187"/>
+    <hyperlink ref="E55" r:id="rId188" location="onrequestpermissionsresult"/>
+    <hyperlink ref="F55" r:id="rId189"/>
+    <hyperlink ref="F11" r:id="rId190"/>
+    <hyperlink ref="F18" r:id="rId191"/>
+    <hyperlink ref="F48" r:id="rId192"/>
+    <hyperlink ref="F49" r:id="rId193"/>
+    <hyperlink ref="E2" r:id="rId194"/>
     <hyperlink ref="E68" r:id="rId195"/>
-    <hyperlink ref="E11" r:id="rId196" location="ChangingTheMenu"/>
-    <hyperlink ref="E18" r:id="rId197" location="ChangingTheMenu"/>
-    <hyperlink ref="E50" r:id="rId198" location="ChangingTheMenu"/>
-    <hyperlink ref="E51" r:id="rId199" location="ChangingTheMenu"/>
-    <hyperlink ref="F12" r:id="rId200" location="!topic/android-platform/G3aN_FekYdg"/>
-    <hyperlink ref="F38" r:id="rId201" location="!topic/android-platform/G3aN_FekYdg"/>
-    <hyperlink ref="E40" r:id="rId202"/>
-    <hyperlink ref="E12" r:id="rId203"/>
-    <hyperlink ref="E83" r:id="rId204" location="onshowfilechooser"/>
-    <hyperlink ref="E90" r:id="rId205" location="onshowfilechooser"/>
-    <hyperlink ref="E64" r:id="rId206" location="onshowcustomview"/>
-    <hyperlink ref="E21" r:id="rId207" location="onshowcustomview"/>
-    <hyperlink ref="F64" r:id="rId208"/>
-    <hyperlink ref="F21" r:id="rId209"/>
-    <hyperlink ref="F7" r:id="rId210"/>
-    <hyperlink ref="E7" r:id="rId211" location="ChangingTheMenu"/>
-    <hyperlink ref="F8" r:id="rId212"/>
-    <hyperlink ref="F51" r:id="rId213"/>
-    <hyperlink ref="E45" r:id="rId214" location="onPermissionRequest(android.webkit.PermissionRequest)"/>
-    <hyperlink ref="E88" r:id="rId215" location="onchange_4"/>
-    <hyperlink ref="E77" r:id="rId216" location="onchange_4"/>
-    <hyperlink ref="F66" r:id="rId217"/>
-    <hyperlink ref="F40" r:id="rId218"/>
-    <hyperlink ref="E66" r:id="rId219"/>
-    <hyperlink ref="E42" r:id="rId220"/>
-    <hyperlink ref="E70" r:id="rId221"/>
-    <hyperlink ref="E10" r:id="rId222"/>
-    <hyperlink ref="E14" r:id="rId223"/>
-    <hyperlink ref="E96" r:id="rId224" location="onscale"/>
-    <hyperlink ref="E41" r:id="rId225"/>
-    <hyperlink ref="E20" r:id="rId226"/>
-    <hyperlink ref="E100" r:id="rId227"/>
-    <hyperlink ref="E97" r:id="rId228"/>
-    <hyperlink ref="E65" r:id="rId229"/>
-    <hyperlink ref="E61" r:id="rId230"/>
-    <hyperlink ref="E16" r:id="rId231" location="onviewstaterestored"/>
-    <hyperlink ref="E19" r:id="rId232"/>
-    <hyperlink ref="E35" r:id="rId233" location="onautofillevent_4"/>
-    <hyperlink ref="E93" r:id="rId234" location="onVisibleBehindCanceled()"/>
-    <hyperlink ref="E89" r:id="rId235" location="setongetplaybackpositionlistener"/>
-    <hyperlink ref="E79" r:id="rId236"/>
-    <hyperlink ref="E80" r:id="rId237"/>
-    <hyperlink ref="E24" r:id="rId238" location="onattach"/>
-    <hyperlink ref="F53" r:id="rId239"/>
-    <hyperlink ref="F54" r:id="rId240"/>
-    <hyperlink ref="E25" r:id="rId241" location="!topic/edx-code/2oU_MbMAxls"/>
-    <hyperlink ref="E75" r:id="rId242" location="onrequestpermissionsresult"/>
-    <hyperlink ref="F75" r:id="rId243"/>
-    <hyperlink ref="E82" r:id="rId244"/>
-    <hyperlink ref="E85" r:id="rId245"/>
+    <hyperlink ref="E67" r:id="rId196"/>
+    <hyperlink ref="E11" r:id="rId197" location="ChangingTheMenu"/>
+    <hyperlink ref="E18" r:id="rId198" location="ChangingTheMenu"/>
+    <hyperlink ref="E48" r:id="rId199" location="ChangingTheMenu"/>
+    <hyperlink ref="E49" r:id="rId200" location="ChangingTheMenu"/>
+    <hyperlink ref="F12" r:id="rId201" location="!topic/android-platform/G3aN_FekYdg"/>
+    <hyperlink ref="F38" r:id="rId202" location="!topic/android-platform/G3aN_FekYdg"/>
+    <hyperlink ref="E38" r:id="rId203"/>
+    <hyperlink ref="E12" r:id="rId204"/>
+    <hyperlink ref="E83" r:id="rId205" location="onshowfilechooser"/>
+    <hyperlink ref="E90" r:id="rId206" location="onshowfilechooser"/>
+    <hyperlink ref="E63" r:id="rId207" location="onshowcustomview"/>
+    <hyperlink ref="E21" r:id="rId208" location="onshowcustomview"/>
+    <hyperlink ref="F63" r:id="rId209"/>
+    <hyperlink ref="F21" r:id="rId210"/>
+    <hyperlink ref="F7" r:id="rId211"/>
+    <hyperlink ref="E7" r:id="rId212" location="ChangingTheMenu"/>
+    <hyperlink ref="F8" r:id="rId213"/>
+    <hyperlink ref="F51" r:id="rId214"/>
+    <hyperlink ref="E43" r:id="rId215" location="onPermissionRequest(android.webkit.PermissionRequest)"/>
+    <hyperlink ref="E88" r:id="rId216" location="onchange_4"/>
+    <hyperlink ref="E76" r:id="rId217" location="onchange_4"/>
+    <hyperlink ref="F65" r:id="rId218"/>
+    <hyperlink ref="F40" r:id="rId219"/>
+    <hyperlink ref="E65" r:id="rId220"/>
+    <hyperlink ref="E40" r:id="rId221"/>
+    <hyperlink ref="E69" r:id="rId222"/>
+    <hyperlink ref="E10" r:id="rId223"/>
+    <hyperlink ref="E14" r:id="rId224"/>
+    <hyperlink ref="E96" r:id="rId225" location="onscale"/>
+    <hyperlink ref="E39" r:id="rId226"/>
+    <hyperlink ref="E20" r:id="rId227"/>
+    <hyperlink ref="E100" r:id="rId228"/>
+    <hyperlink ref="E97" r:id="rId229"/>
+    <hyperlink ref="E64" r:id="rId230"/>
+    <hyperlink ref="E60" r:id="rId231"/>
+    <hyperlink ref="E16" r:id="rId232" location="onviewstaterestored"/>
+    <hyperlink ref="E19" r:id="rId233"/>
+    <hyperlink ref="E33" r:id="rId234" location="onautofillevent_4"/>
+    <hyperlink ref="E93" r:id="rId235" location="onVisibleBehindCanceled()"/>
+    <hyperlink ref="E89" r:id="rId236" location="setongetplaybackpositionlistener"/>
+    <hyperlink ref="E78" r:id="rId237"/>
+    <hyperlink ref="E79" r:id="rId238"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId246"/>
+  <legacyDrawing r:id="rId239"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
continue to implement the execution order
</commit_message>
<xml_diff>
--- a/empirical.xlsx
+++ b/empirical.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huanghuaxun/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huanghuaxun/Documents/GitHub/cideranalyzer.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>